<commit_message>
adding old table structure
</commit_message>
<xml_diff>
--- a/docs/TableStructure.xlsx
+++ b/docs/TableStructure.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
-    <sheet name="New Table Structure" sheetId="2" r:id="rId2"/>
+    <sheet name="Old Table Structure" sheetId="3" r:id="rId2"/>
+    <sheet name="New Table Structure" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="320">
   <si>
     <t>Existing Database Structure</t>
   </si>
@@ -1241,12 +1242,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1445,24 +1452,44 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1471,6 +1498,900 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8859520" y="3180080"/>
+          <a:ext cx="1107440" cy="599440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6644640" y="1005840"/>
+          <a:ext cx="1097280" cy="2001520"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6644640" y="3017520"/>
+          <a:ext cx="1097280" cy="619760"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4429760" y="3474720"/>
+          <a:ext cx="1107440" cy="1229360"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Connector 26"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7752080" y="3169920"/>
+          <a:ext cx="2214880" cy="4744720"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>843280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>955040</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3053080" y="492760"/>
+          <a:ext cx="1216660" cy="10160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>843280</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>955040</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Connector 28"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3053080" y="863600"/>
+          <a:ext cx="1216660" cy="10160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>955040</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3073400" y="1275080"/>
+          <a:ext cx="1196340" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>843280</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>955040</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Connector 30"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3053080" y="1064260"/>
+          <a:ext cx="1216660" cy="10160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11084560" y="883920"/>
+          <a:ext cx="3312160" cy="4907280"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1087120</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11054080" y="2235200"/>
+          <a:ext cx="3352800" cy="3566160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Connector 44"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11064240" y="3769360"/>
+          <a:ext cx="3322320" cy="2042160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Straight Connector 47"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11064240" y="5019040"/>
+          <a:ext cx="3322320" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Connector 50"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11064240" y="5811520"/>
+          <a:ext cx="3322320" cy="568960"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Connector 53"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11084560" y="3159760"/>
+          <a:ext cx="1097280" cy="4196080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Straight Connector 56"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13289280" y="7914640"/>
+          <a:ext cx="1097280" cy="792480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Connector 57"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13289280" y="8107680"/>
+          <a:ext cx="1107440" cy="375920"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>568960</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>10160</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>71120</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Straight Arrow Connector 68"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13858240" y="5781040"/>
+          <a:ext cx="3159760" cy="1910080"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>568960</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="Straight Connector 71"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13858240" y="7680960"/>
+          <a:ext cx="10160" cy="599440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Straight Arrow Connector 75"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18115280" y="5791200"/>
+          <a:ext cx="1107440" cy="1188720"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1812,13 +2733,13 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1859,13 +2780,13 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -2214,13 +3135,13 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:fillRef>
         <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -2556,8 +3477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L988"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -2567,7 +3488,7 @@
     <col min="9" max="9" width="57.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1">
+    <row r="1" spans="1:11" ht="12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +3505,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1">
+    <row r="2" spans="1:11" ht="12">
       <c r="A2" s="5"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2597,7 +3518,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1">
+    <row r="3" spans="1:11" ht="12">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2612,7 +3533,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+    <row r="4" spans="1:11" ht="12">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
@@ -2627,30 +3548,30 @@
       <c r="J4" s="14"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1">
+    <row r="5" spans="1:11" ht="12">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="16"/>
-      <c r="C5" s="137"/>
-      <c r="D5" s="135"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="139"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="141" t="s">
+      <c r="F5" s="140" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="135"/>
+      <c r="G5" s="139"/>
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
       <c r="J5" s="14"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="142" t="s">
+    <row r="6" spans="1:11" ht="12">
+      <c r="A6" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="135"/>
-      <c r="C6" s="135"/>
-      <c r="D6" s="135"/>
+      <c r="B6" s="139"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="139"/>
       <c r="E6" s="18"/>
       <c r="F6" s="6"/>
       <c r="G6" s="2"/>
@@ -2659,7 +3580,7 @@
       <c r="J6" s="14"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1">
+    <row r="7" spans="1:11" ht="12">
       <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
@@ -2674,7 +3595,7 @@
       <c r="J7" s="24"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1">
+    <row r="8" spans="1:11" ht="12">
       <c r="A8" s="5"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2687,7 +3608,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1">
+    <row r="9" spans="1:11" ht="48">
       <c r="A9" s="25" t="s">
         <v>8</v>
       </c>
@@ -2704,7 +3625,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1">
+    <row r="10" spans="1:11" ht="12">
       <c r="A10" s="28" t="s">
         <v>10</v>
       </c>
@@ -2725,7 +3646,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:11" ht="12">
       <c r="A11" s="30" t="s">
         <v>14</v>
       </c>
@@ -2744,7 +3665,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1">
+    <row r="12" spans="1:11" ht="12">
       <c r="A12" s="30" t="s">
         <v>16</v>
       </c>
@@ -2763,7 +3684,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1">
+    <row r="13" spans="1:11" ht="12">
       <c r="A13" s="30" t="s">
         <v>19</v>
       </c>
@@ -2782,7 +3703,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1">
+    <row r="14" spans="1:11" ht="12">
       <c r="A14" s="30" t="s">
         <v>21</v>
       </c>
@@ -2801,7 +3722,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1">
+    <row r="15" spans="1:11" ht="12">
       <c r="A15" s="30" t="s">
         <v>23</v>
       </c>
@@ -2820,7 +3741,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1">
+    <row r="16" spans="1:11" ht="12">
       <c r="A16" s="30" t="s">
         <v>26</v>
       </c>
@@ -2839,7 +3760,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1">
+    <row r="17" spans="1:11" ht="12">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2852,11 +3773,11 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1">
+    <row r="18" spans="1:11" ht="48">
       <c r="A18" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="135"/>
+      <c r="B18" s="139"/>
       <c r="C18" s="26"/>
       <c r="D18" s="27" t="s">
         <v>9</v>
@@ -2869,7 +3790,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1">
+    <row r="19" spans="1:11" ht="12">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -2890,7 +3811,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1">
+    <row r="20" spans="1:11" ht="12">
       <c r="A20" s="30" t="s">
         <v>14</v>
       </c>
@@ -2911,7 +3832,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1">
+    <row r="21" spans="1:11" ht="12">
       <c r="A21" s="30" t="s">
         <v>31</v>
       </c>
@@ -2930,7 +3851,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1">
+    <row r="22" spans="1:11" ht="12">
       <c r="A22" s="30" t="s">
         <v>26</v>
       </c>
@@ -2949,7 +3870,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1">
+    <row r="23" spans="1:11" ht="12">
       <c r="A23" s="30" t="s">
         <v>35</v>
       </c>
@@ -2968,7 +3889,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1">
+    <row r="24" spans="1:11" ht="12">
       <c r="A24" s="30" t="s">
         <v>37</v>
       </c>
@@ -2987,7 +3908,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1">
+    <row r="25" spans="1:11" ht="12">
       <c r="A25" s="30" t="s">
         <v>40</v>
       </c>
@@ -3006,7 +3927,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1">
+    <row r="26" spans="1:11" ht="12">
       <c r="A26" s="30" t="s">
         <v>41</v>
       </c>
@@ -3025,7 +3946,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1">
+    <row r="27" spans="1:11" ht="12">
       <c r="A27" s="30" t="s">
         <v>42</v>
       </c>
@@ -3044,7 +3965,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1">
+    <row r="28" spans="1:11" ht="12">
       <c r="A28" s="30" t="s">
         <v>43</v>
       </c>
@@ -3063,7 +3984,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1">
+    <row r="29" spans="1:11" ht="12">
       <c r="A29" s="30" t="s">
         <v>45</v>
       </c>
@@ -3082,7 +4003,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1">
+    <row r="30" spans="1:11" ht="12">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3095,11 +4016,11 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A31" s="134" t="s">
+    <row r="31" spans="1:11" ht="96">
+      <c r="A31" s="146" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="135"/>
+      <c r="B31" s="139"/>
       <c r="C31" s="2"/>
       <c r="D31" s="33" t="s">
         <v>49</v>
@@ -3116,7 +4037,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1">
+    <row r="32" spans="1:11" ht="12">
       <c r="A32" s="36" t="s">
         <v>10</v>
       </c>
@@ -3145,7 +4066,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1">
+    <row r="33" spans="1:11" ht="12">
       <c r="A33" s="38" t="s">
         <v>14</v>
       </c>
@@ -3174,7 +4095,7 @@
       <c r="J33" s="43"/>
       <c r="K33" s="43"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1">
+    <row r="34" spans="1:11" ht="12">
       <c r="A34" s="44" t="s">
         <v>31</v>
       </c>
@@ -3201,7 +4122,7 @@
       <c r="J34" s="52"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+    <row r="35" spans="1:11" ht="12">
       <c r="A35" s="43" t="s">
         <v>57</v>
       </c>
@@ -3226,7 +4147,7 @@
       <c r="J35" s="33"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1">
+    <row r="36" spans="1:11" ht="12">
       <c r="A36" s="43" t="s">
         <v>59</v>
       </c>
@@ -3251,7 +4172,7 @@
       <c r="J36" s="33"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1">
+    <row r="37" spans="1:11" ht="12">
       <c r="A37" s="43" t="s">
         <v>61</v>
       </c>
@@ -3276,7 +4197,7 @@
       <c r="J37" s="33"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1">
+    <row r="38" spans="1:11" ht="12">
       <c r="A38" s="55" t="s">
         <v>63</v>
       </c>
@@ -3301,7 +4222,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1">
+    <row r="39" spans="1:11" ht="12">
       <c r="A39" s="55" t="s">
         <v>66</v>
       </c>
@@ -3326,7 +4247,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1">
+    <row r="40" spans="1:11" ht="12">
       <c r="A40" s="55" t="s">
         <v>67</v>
       </c>
@@ -3351,7 +4272,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1">
+    <row r="41" spans="1:11" ht="12">
       <c r="A41" s="55" t="s">
         <v>68</v>
       </c>
@@ -3376,7 +4297,7 @@
       <c r="J41" s="47"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1">
+    <row r="42" spans="1:11" ht="12">
       <c r="A42" s="55" t="s">
         <v>70</v>
       </c>
@@ -3401,7 +4322,7 @@
       <c r="J42" s="47"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1">
+    <row r="43" spans="1:11" ht="12">
       <c r="A43" s="55" t="s">
         <v>71</v>
       </c>
@@ -3426,7 +4347,7 @@
       <c r="J43" s="47"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1">
+    <row r="44" spans="1:11" ht="12">
       <c r="A44" s="55" t="s">
         <v>72</v>
       </c>
@@ -3451,7 +4372,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1">
+    <row r="45" spans="1:11" ht="12">
       <c r="A45" s="55" t="s">
         <v>75</v>
       </c>
@@ -3476,7 +4397,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1">
+    <row r="46" spans="1:11" ht="12">
       <c r="A46" s="55" t="s">
         <v>78</v>
       </c>
@@ -3501,7 +4422,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1">
+    <row r="47" spans="1:11" ht="12">
       <c r="A47" s="55" t="s">
         <v>80</v>
       </c>
@@ -3526,7 +4447,7 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1">
+    <row r="48" spans="1:11" ht="12">
       <c r="A48" s="55" t="s">
         <v>82</v>
       </c>
@@ -3551,7 +4472,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1">
+    <row r="49" spans="1:11" ht="12">
       <c r="A49" s="55" t="s">
         <v>84</v>
       </c>
@@ -3576,7 +4497,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" ht="15.75" customHeight="1">
+    <row r="50" spans="1:11" ht="12">
       <c r="A50" s="55" t="s">
         <v>86</v>
       </c>
@@ -3601,7 +4522,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" ht="15.75" customHeight="1">
+    <row r="51" spans="1:11" ht="12">
       <c r="A51" s="43" t="s">
         <v>87</v>
       </c>
@@ -3625,7 +4546,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" ht="15.75" customHeight="1">
+    <row r="52" spans="1:11" ht="12">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -3633,7 +4554,7 @@
       <c r="E52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" ht="15.75" customHeight="1">
+    <row r="53" spans="1:11" ht="12">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3646,11 +4567,11 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A54" s="134" t="s">
+    <row r="54" spans="1:11" ht="84">
+      <c r="A54" s="146" t="s">
         <v>89</v>
       </c>
-      <c r="B54" s="135"/>
+      <c r="B54" s="139"/>
       <c r="C54" s="2"/>
       <c r="D54" s="33" t="s">
         <v>90</v>
@@ -3667,7 +4588,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:11" ht="15.75" customHeight="1">
+    <row r="55" spans="1:11" ht="12">
       <c r="A55" s="36" t="s">
         <v>10</v>
       </c>
@@ -3696,7 +4617,7 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" ht="15.75" customHeight="1">
+    <row r="56" spans="1:11" ht="12">
       <c r="A56" s="38" t="s">
         <v>14</v>
       </c>
@@ -3725,7 +4646,7 @@
       <c r="J56" s="43"/>
       <c r="K56" s="43"/>
     </row>
-    <row r="57" spans="1:11" ht="15.75" customHeight="1">
+    <row r="57" spans="1:11" ht="12">
       <c r="A57" s="64" t="s">
         <v>97</v>
       </c>
@@ -3748,7 +4669,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" ht="15.75" customHeight="1">
+    <row r="58" spans="1:11" ht="12">
       <c r="A58" s="64" t="s">
         <v>99</v>
       </c>
@@ -3763,17 +4684,17 @@
       <c r="F58" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="G58" s="136" t="s">
+      <c r="G58" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H58" s="135"/>
+      <c r="H58" s="139"/>
       <c r="I58" s="33" t="s">
         <v>103</v>
       </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" ht="15.75" customHeight="1">
+    <row r="59" spans="1:11" ht="12">
       <c r="A59" s="43" t="s">
         <v>26</v>
       </c>
@@ -3787,17 +4708,17 @@
       <c r="F59" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="G59" s="136" t="s">
+      <c r="G59" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H59" s="135"/>
+      <c r="H59" s="139"/>
       <c r="I59" s="33" t="s">
         <v>106</v>
       </c>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
     </row>
-    <row r="60" spans="1:11" ht="15.75" customHeight="1">
+    <row r="60" spans="1:11" ht="12">
       <c r="A60" s="64" t="s">
         <v>107</v>
       </c>
@@ -3812,17 +4733,17 @@
       <c r="F60" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="G60" s="136" t="s">
+      <c r="G60" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H60" s="135"/>
+      <c r="H60" s="139"/>
       <c r="I60" s="33" t="s">
         <v>110</v>
       </c>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" ht="15.75" customHeight="1">
+    <row r="61" spans="1:11" ht="12">
       <c r="A61" s="64" t="s">
         <v>111</v>
       </c>
@@ -3847,7 +4768,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:11" ht="15.75" customHeight="1">
+    <row r="62" spans="1:11" ht="12">
       <c r="A62" s="64" t="s">
         <v>116</v>
       </c>
@@ -3862,17 +4783,17 @@
       <c r="F62" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="G62" s="136" t="s">
+      <c r="G62" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H62" s="135"/>
+      <c r="H62" s="139"/>
       <c r="I62" s="33" t="s">
         <v>118</v>
       </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" ht="15.75" customHeight="1">
+    <row r="63" spans="1:11" ht="12">
       <c r="A63" s="64" t="s">
         <v>119</v>
       </c>
@@ -3887,7 +4808,7 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" ht="15.75" customHeight="1">
+    <row r="64" spans="1:11" ht="48">
       <c r="A64" s="64" t="s">
         <v>120</v>
       </c>
@@ -3910,7 +4831,7 @@
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" ht="15.75" customHeight="1">
+    <row r="65" spans="1:11" ht="12">
       <c r="A65" s="64" t="s">
         <v>123</v>
       </c>
@@ -3937,7 +4858,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" ht="15.75" customHeight="1">
+    <row r="66" spans="1:11" ht="12">
       <c r="A66" s="64" t="s">
         <v>126</v>
       </c>
@@ -3964,7 +4885,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" ht="15.75" customHeight="1">
+    <row r="67" spans="1:11" ht="12">
       <c r="A67" s="43" t="s">
         <v>101</v>
       </c>
@@ -3978,17 +4899,17 @@
       <c r="F67" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="G67" s="136" t="s">
+      <c r="G67" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H67" s="135"/>
+      <c r="H67" s="139"/>
       <c r="I67" s="33" t="s">
         <v>100</v>
       </c>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" ht="15.75" customHeight="1">
+    <row r="68" spans="1:11" ht="12">
       <c r="A68" s="64" t="s">
         <v>127</v>
       </c>
@@ -4003,17 +4924,17 @@
       <c r="F68" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="G68" s="136" t="s">
+      <c r="G68" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H68" s="135"/>
+      <c r="H68" s="139"/>
       <c r="I68" s="33" t="s">
         <v>100</v>
       </c>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
     </row>
-    <row r="69" spans="1:11" ht="15.75" customHeight="1">
+    <row r="69" spans="1:11" ht="12">
       <c r="A69" s="43" t="s">
         <v>16</v>
       </c>
@@ -4027,17 +4948,17 @@
       <c r="F69" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="G69" s="136" t="s">
+      <c r="G69" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H69" s="135"/>
+      <c r="H69" s="139"/>
       <c r="I69" s="33" t="s">
         <v>100</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" ht="15.75" customHeight="1">
+    <row r="70" spans="1:11" ht="12">
       <c r="A70" s="43" t="s">
         <v>105</v>
       </c>
@@ -4061,7 +4982,7 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" ht="15.75" customHeight="1">
+    <row r="71" spans="1:11" ht="12">
       <c r="A71" s="43" t="s">
         <v>108</v>
       </c>
@@ -4075,17 +4996,17 @@
       <c r="F71" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="G71" s="136" t="s">
+      <c r="G71" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H71" s="135"/>
+      <c r="H71" s="139"/>
       <c r="I71" s="33" t="s">
         <v>118</v>
       </c>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" ht="15.75" customHeight="1">
+    <row r="72" spans="1:11" ht="12">
       <c r="A72" s="64" t="s">
         <v>130</v>
       </c>
@@ -4110,7 +5031,7 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" ht="15.75" customHeight="1">
+    <row r="73" spans="1:11" ht="12">
       <c r="A73" s="64" t="s">
         <v>134</v>
       </c>
@@ -4125,17 +5046,17 @@
       <c r="F73" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="G73" s="136" t="s">
+      <c r="G73" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="H73" s="135"/>
+      <c r="H73" s="139"/>
       <c r="I73" s="33" t="s">
         <v>135</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
-    <row r="74" spans="1:11" ht="15.75" customHeight="1">
+    <row r="74" spans="1:11" ht="12">
       <c r="A74" s="64" t="s">
         <v>136</v>
       </c>
@@ -4160,14 +5081,14 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" ht="15.75" customHeight="1">
+    <row r="75" spans="1:11" ht="12">
       <c r="A75" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B75" s="136" t="s">
+      <c r="B75" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="C75" s="135"/>
+      <c r="C75" s="139"/>
       <c r="D75" s="33" t="s">
         <v>115</v>
       </c>
@@ -4175,14 +5096,14 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" ht="15.75" customHeight="1">
+    <row r="76" spans="1:11" ht="12">
       <c r="A76" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="B76" s="137" t="s">
+      <c r="B76" s="142" t="s">
         <v>139</v>
       </c>
-      <c r="C76" s="135"/>
+      <c r="C76" s="139"/>
       <c r="D76" s="69" t="s">
         <v>140</v>
       </c>
@@ -4190,7 +5111,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" ht="15.75" customHeight="1">
+    <row r="77" spans="1:11" ht="12">
       <c r="A77" s="43" t="s">
         <v>29</v>
       </c>
@@ -4204,7 +5125,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" ht="15.75" customHeight="1">
+    <row r="78" spans="1:11" ht="12">
       <c r="A78" s="64" t="s">
         <v>21</v>
       </c>
@@ -4219,7 +5140,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" ht="15.75" customHeight="1">
+    <row r="79" spans="1:11" ht="12">
       <c r="A79" s="43" t="s">
         <v>117</v>
       </c>
@@ -4233,7 +5154,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" ht="15.75" customHeight="1">
+    <row r="80" spans="1:11" ht="12">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4246,7 +5167,7 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" ht="15.75" customHeight="1">
+    <row r="81" spans="1:11" ht="12">
       <c r="A81" s="32" t="s">
         <v>144</v>
       </c>
@@ -4267,7 +5188,7 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" ht="15.75" customHeight="1">
+    <row r="82" spans="1:11" ht="12">
       <c r="A82" s="36" t="s">
         <v>10</v>
       </c>
@@ -4296,7 +5217,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" ht="15.75" customHeight="1">
+    <row r="83" spans="1:11" ht="12">
       <c r="A83" s="38" t="s">
         <v>14</v>
       </c>
@@ -4323,7 +5244,7 @@
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
     </row>
-    <row r="84" spans="1:11" ht="15.75" customHeight="1">
+    <row r="84" spans="1:11" ht="12">
       <c r="A84" s="64" t="s">
         <v>97</v>
       </c>
@@ -4350,14 +5271,14 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" ht="15.75" customHeight="1">
+    <row r="85" spans="1:11" ht="12">
       <c r="A85" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B85" s="138" t="s">
+      <c r="B85" s="147" t="s">
         <v>157</v>
       </c>
-      <c r="C85" s="135"/>
+      <c r="C85" s="139"/>
       <c r="D85" s="90" t="s">
         <v>28</v>
       </c>
@@ -4365,17 +5286,17 @@
       <c r="F85" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="G85" s="136" t="s">
+      <c r="G85" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H85" s="135"/>
+      <c r="H85" s="139"/>
       <c r="I85" s="33" t="s">
         <v>164</v>
       </c>
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" ht="15.75" customHeight="1">
+    <row r="86" spans="1:11" ht="12">
       <c r="A86" s="43" t="s">
         <v>101</v>
       </c>
@@ -4400,7 +5321,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" ht="15.75" customHeight="1">
+    <row r="87" spans="1:11" ht="12">
       <c r="A87" s="92" t="s">
         <v>134</v>
       </c>
@@ -4415,17 +5336,17 @@
       <c r="F87" s="54" t="s">
         <v>168</v>
       </c>
-      <c r="G87" s="136" t="s">
+      <c r="G87" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H87" s="135"/>
+      <c r="H87" s="139"/>
       <c r="I87" s="33" t="s">
         <v>174</v>
       </c>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" ht="15.75" customHeight="1">
+    <row r="88" spans="1:11" ht="60">
       <c r="A88" s="92" t="s">
         <v>136</v>
       </c>
@@ -4440,24 +5361,24 @@
       <c r="F88" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="G88" s="136" t="s">
+      <c r="G88" s="138" t="s">
         <v>102</v>
       </c>
-      <c r="H88" s="135"/>
+      <c r="H88" s="139"/>
       <c r="I88" s="33" t="s">
         <v>175</v>
       </c>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" ht="15.75" customHeight="1">
+    <row r="89" spans="1:11" ht="24">
       <c r="A89" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B89" s="136" t="s">
+      <c r="B89" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="C89" s="135"/>
+      <c r="C89" s="139"/>
       <c r="D89" s="33" t="s">
         <v>115</v>
       </c>
@@ -4465,17 +5386,17 @@
       <c r="F89" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="G89" s="140" t="s">
+      <c r="G89" s="144" t="s">
         <v>102</v>
       </c>
-      <c r="H89" s="135"/>
+      <c r="H89" s="139"/>
       <c r="I89" s="100" t="s">
         <v>181</v>
       </c>
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" ht="15.75" customHeight="1">
+    <row r="90" spans="1:11" ht="12">
       <c r="A90" s="43" t="s">
         <v>168</v>
       </c>
@@ -4491,7 +5412,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" ht="15.75" customHeight="1">
+    <row r="91" spans="1:11" ht="48">
       <c r="A91" s="43" t="s">
         <v>169</v>
       </c>
@@ -4507,7 +5428,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" ht="15.75" customHeight="1">
+    <row r="92" spans="1:11" ht="24">
       <c r="A92" s="55" t="s">
         <v>178</v>
       </c>
@@ -4526,7 +5447,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" ht="15.75" customHeight="1">
+    <row r="93" spans="1:11" ht="12">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4539,11 +5460,11 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A94" s="134" t="s">
+    <row r="94" spans="1:11" ht="48">
+      <c r="A94" s="146" t="s">
         <v>189</v>
       </c>
-      <c r="B94" s="135"/>
+      <c r="B94" s="139"/>
       <c r="C94" s="2"/>
       <c r="D94" s="33" t="s">
         <v>190</v>
@@ -4560,7 +5481,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" ht="15.75" customHeight="1">
+    <row r="95" spans="1:11" ht="12">
       <c r="A95" s="36" t="s">
         <v>10</v>
       </c>
@@ -4589,7 +5510,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" ht="15.75" customHeight="1">
+    <row r="96" spans="1:11" ht="12">
       <c r="A96" s="38" t="s">
         <v>14</v>
       </c>
@@ -4618,7 +5539,7 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" ht="15.75" customHeight="1">
+    <row r="97" spans="1:11" ht="12">
       <c r="A97" s="64" t="s">
         <v>206</v>
       </c>
@@ -4643,7 +5564,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" ht="15.75" customHeight="1">
+    <row r="98" spans="1:11" ht="12">
       <c r="A98" s="43" t="s">
         <v>141</v>
       </c>
@@ -4668,7 +5589,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" ht="15.75" customHeight="1">
+    <row r="99" spans="1:11" ht="12">
       <c r="A99" s="43" t="s">
         <v>113</v>
       </c>
@@ -4686,7 +5607,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" ht="15.75" customHeight="1">
+    <row r="100" spans="1:11" ht="12">
       <c r="A100" s="64" t="s">
         <v>138</v>
       </c>
@@ -4704,7 +5625,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" ht="15.75" customHeight="1">
+    <row r="101" spans="1:11" ht="12">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4717,11 +5638,11 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A102" s="134" t="s">
+    <row r="102" spans="1:11" ht="48">
+      <c r="A102" s="146" t="s">
         <v>210</v>
       </c>
-      <c r="B102" s="135"/>
+      <c r="B102" s="139"/>
       <c r="C102" s="2"/>
       <c r="D102" s="33" t="s">
         <v>211</v>
@@ -4738,7 +5659,7 @@
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
     </row>
-    <row r="103" spans="1:11" ht="15.75" customHeight="1">
+    <row r="103" spans="1:11" ht="12">
       <c r="A103" s="36" t="s">
         <v>10</v>
       </c>
@@ -4767,7 +5688,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" ht="15.75" customHeight="1">
+    <row r="104" spans="1:11" ht="12">
       <c r="A104" s="39" t="s">
         <v>14</v>
       </c>
@@ -4796,7 +5717,7 @@
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
     </row>
-    <row r="105" spans="1:11" ht="15.75" customHeight="1">
+    <row r="105" spans="1:11" ht="12">
       <c r="A105" s="64" t="s">
         <v>206</v>
       </c>
@@ -4821,7 +5742,7 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" ht="15.75" customHeight="1">
+    <row r="106" spans="1:11" ht="12">
       <c r="A106" s="43" t="s">
         <v>215</v>
       </c>
@@ -4845,7 +5766,7 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" ht="15.75" customHeight="1">
+    <row r="107" spans="1:11" ht="12">
       <c r="A107" s="43" t="s">
         <v>217</v>
       </c>
@@ -4869,7 +5790,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="1:11" ht="15.75" customHeight="1">
+    <row r="108" spans="1:11" ht="12">
       <c r="A108" s="43" t="s">
         <v>113</v>
       </c>
@@ -4887,7 +5808,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" ht="15.75" customHeight="1">
+    <row r="109" spans="1:11" ht="12">
       <c r="A109" s="64" t="s">
         <v>138</v>
       </c>
@@ -4905,7 +5826,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="1:11" ht="15.75" customHeight="1">
+    <row r="110" spans="1:11" ht="12">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4918,11 +5839,11 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A111" s="134" t="s">
+    <row r="111" spans="1:11" ht="72">
+      <c r="A111" s="146" t="s">
         <v>218</v>
       </c>
-      <c r="B111" s="135"/>
+      <c r="B111" s="139"/>
       <c r="C111" s="2"/>
       <c r="D111" s="33" t="s">
         <v>219</v>
@@ -4939,7 +5860,7 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="1:11" ht="15.75" customHeight="1">
+    <row r="112" spans="1:11" ht="12">
       <c r="A112" s="36" t="s">
         <v>10</v>
       </c>
@@ -4968,7 +5889,7 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="1:11" ht="15.75" customHeight="1">
+    <row r="113" spans="1:11" ht="12">
       <c r="A113" s="39" t="s">
         <v>14</v>
       </c>
@@ -4997,7 +5918,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="1:11" ht="15.75" customHeight="1">
+    <row r="114" spans="1:11" ht="12">
       <c r="A114" s="64" t="s">
         <v>97</v>
       </c>
@@ -5022,7 +5943,7 @@
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
     </row>
-    <row r="115" spans="1:11" ht="15.75" customHeight="1">
+    <row r="115" spans="1:11" ht="12">
       <c r="A115" s="43" t="s">
         <v>16</v>
       </c>
@@ -5046,7 +5967,7 @@
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="1:11" ht="15.75" customHeight="1">
+    <row r="116" spans="1:11" ht="24">
       <c r="A116" s="43" t="s">
         <v>165</v>
       </c>
@@ -5070,7 +5991,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="1:11" ht="15.75" customHeight="1">
+    <row r="117" spans="1:11" ht="12">
       <c r="A117" s="43" t="s">
         <v>166</v>
       </c>
@@ -5094,7 +6015,7 @@
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="1:11" ht="15.75" customHeight="1">
+    <row r="118" spans="1:11" ht="12">
       <c r="A118" s="43" t="s">
         <v>113</v>
       </c>
@@ -5112,7 +6033,7 @@
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="1:11" ht="15.75" customHeight="1">
+    <row r="119" spans="1:11" ht="12">
       <c r="A119" s="64" t="s">
         <v>138</v>
       </c>
@@ -5130,7 +6051,7 @@
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="1:11" ht="15.75" customHeight="1">
+    <row r="120" spans="1:11" ht="12">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5143,11 +6064,11 @@
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A121" s="134" t="s">
+    <row r="121" spans="1:11" ht="36">
+      <c r="A121" s="146" t="s">
         <v>224</v>
       </c>
-      <c r="B121" s="135"/>
+      <c r="B121" s="139"/>
       <c r="C121" s="2"/>
       <c r="D121" s="33" t="s">
         <v>225</v>
@@ -5164,7 +6085,7 @@
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="1:11" ht="15.75" customHeight="1">
+    <row r="122" spans="1:11" ht="12">
       <c r="A122" s="36" t="s">
         <v>10</v>
       </c>
@@ -5193,7 +6114,7 @@
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1">
+    <row r="123" spans="1:11" ht="12">
       <c r="A123" s="38" t="s">
         <v>14</v>
       </c>
@@ -5222,7 +6143,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="1:11" ht="15.75" customHeight="1">
+    <row r="124" spans="1:11" ht="12">
       <c r="A124" s="55" t="s">
         <v>109</v>
       </c>
@@ -5246,7 +6167,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="1:11" ht="15.75" customHeight="1">
+    <row r="125" spans="1:11" ht="12">
       <c r="A125" s="43" t="s">
         <v>21</v>
       </c>
@@ -5270,7 +6191,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="1:11" ht="15.75" customHeight="1">
+    <row r="126" spans="1:11" ht="12">
       <c r="A126" s="43" t="s">
         <v>113</v>
       </c>
@@ -5294,7 +6215,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="1:11" ht="15.75" customHeight="1">
+    <row r="127" spans="1:11" ht="12">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -5307,11 +6228,11 @@
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A128" s="134" t="s">
+    <row r="128" spans="1:11" ht="36">
+      <c r="A128" s="146" t="s">
         <v>230</v>
       </c>
-      <c r="B128" s="135"/>
+      <c r="B128" s="139"/>
       <c r="C128" s="2"/>
       <c r="D128" s="33" t="s">
         <v>231</v>
@@ -5328,7 +6249,7 @@
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="1:11" ht="15.75" customHeight="1">
+    <row r="129" spans="1:11" ht="12">
       <c r="A129" s="36" t="s">
         <v>10</v>
       </c>
@@ -5357,7 +6278,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="1:11" ht="15.75" customHeight="1">
+    <row r="130" spans="1:11" ht="12">
       <c r="A130" s="38" t="s">
         <v>14</v>
       </c>
@@ -5386,7 +6307,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="1:11" ht="15.75" customHeight="1">
+    <row r="131" spans="1:11" ht="12">
       <c r="A131" s="64" t="s">
         <v>109</v>
       </c>
@@ -5401,24 +6322,24 @@
       <c r="F131" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="G131" s="136" t="s">
+      <c r="G131" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="H131" s="135"/>
+      <c r="H131" s="139"/>
       <c r="I131" s="33" t="s">
         <v>229</v>
       </c>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="1:11" ht="15.75" customHeight="1">
+    <row r="132" spans="1:11" ht="12">
       <c r="A132" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B132" s="136" t="s">
+      <c r="B132" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="C132" s="135"/>
+      <c r="C132" s="139"/>
       <c r="D132" s="33" t="s">
         <v>229</v>
       </c>
@@ -5426,24 +6347,24 @@
       <c r="F132" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="G132" s="136" t="s">
+      <c r="G132" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="H132" s="135"/>
+      <c r="H132" s="139"/>
       <c r="I132" s="33" t="s">
         <v>115</v>
       </c>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="1:11" ht="15.75" customHeight="1">
+    <row r="133" spans="1:11" ht="12">
       <c r="A133" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B133" s="136" t="s">
+      <c r="B133" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="C133" s="135"/>
+      <c r="C133" s="139"/>
       <c r="D133" s="33" t="s">
         <v>115</v>
       </c>
@@ -5452,7 +6373,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="1:11" ht="15.75" customHeight="1">
+    <row r="134" spans="1:11" ht="12">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -5465,7 +6386,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="1:11" ht="15.75" customHeight="1">
+    <row r="135" spans="1:11" ht="12">
       <c r="A135" s="25" t="s">
         <v>235</v>
       </c>
@@ -5482,7 +6403,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="1:11" ht="15.75" customHeight="1">
+    <row r="136" spans="1:11" ht="12">
       <c r="A136" s="28" t="s">
         <v>10</v>
       </c>
@@ -5503,7 +6424,7 @@
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="1:11" ht="15.75" customHeight="1">
+    <row r="137" spans="1:11" ht="12">
       <c r="A137" s="30" t="s">
         <v>26</v>
       </c>
@@ -5522,7 +6443,7 @@
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="1:11" ht="15.75" customHeight="1">
+    <row r="138" spans="1:11" ht="12">
       <c r="A138" s="30" t="s">
         <v>237</v>
       </c>
@@ -5539,7 +6460,7 @@
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="1:11" ht="15.75" customHeight="1">
+    <row r="139" spans="1:11" ht="12">
       <c r="A139" s="30" t="s">
         <v>203</v>
       </c>
@@ -5556,7 +6477,7 @@
       <c r="J139" s="2"/>
       <c r="K139" s="2"/>
     </row>
-    <row r="140" spans="1:11" ht="15.75" customHeight="1">
+    <row r="140" spans="1:11" ht="12">
       <c r="A140" s="30" t="s">
         <v>29</v>
       </c>
@@ -5573,7 +6494,7 @@
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
     </row>
-    <row r="141" spans="1:11" ht="15.75" customHeight="1">
+    <row r="141" spans="1:11" ht="12">
       <c r="A141" s="30" t="s">
         <v>101</v>
       </c>
@@ -5590,7 +6511,7 @@
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
     </row>
-    <row r="142" spans="1:11" ht="15.75" customHeight="1">
+    <row r="142" spans="1:11" ht="12">
       <c r="A142" s="30" t="s">
         <v>239</v>
       </c>
@@ -5607,7 +6528,7 @@
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
     </row>
-    <row r="143" spans="1:11" ht="15.75" customHeight="1">
+    <row r="143" spans="1:11" ht="12">
       <c r="A143" s="30" t="s">
         <v>16</v>
       </c>
@@ -5624,7 +6545,7 @@
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
     </row>
-    <row r="144" spans="1:11" ht="15.75" customHeight="1">
+    <row r="144" spans="1:11" ht="12">
       <c r="A144" s="30" t="s">
         <v>240</v>
       </c>
@@ -5641,7 +6562,7 @@
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
     </row>
-    <row r="145" spans="1:11" ht="15.75" customHeight="1">
+    <row r="145" spans="1:11" ht="12">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -5654,11 +6575,11 @@
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
     </row>
-    <row r="146" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A146" s="134" t="s">
+    <row r="146" spans="1:11" ht="36">
+      <c r="A146" s="146" t="s">
         <v>241</v>
       </c>
-      <c r="B146" s="135"/>
+      <c r="B146" s="139"/>
       <c r="C146" s="2"/>
       <c r="D146" s="33" t="s">
         <v>242</v>
@@ -5675,7 +6596,7 @@
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
     </row>
-    <row r="147" spans="1:11" ht="15.75" customHeight="1">
+    <row r="147" spans="1:11" ht="12">
       <c r="A147" s="36" t="s">
         <v>10</v>
       </c>
@@ -5704,7 +6625,7 @@
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
     </row>
-    <row r="148" spans="1:11" ht="15.75" customHeight="1">
+    <row r="148" spans="1:11" ht="12">
       <c r="A148" s="39" t="s">
         <v>14</v>
       </c>
@@ -5733,7 +6654,7 @@
       <c r="J148" s="2"/>
       <c r="K148" s="2"/>
     </row>
-    <row r="149" spans="1:11" ht="15.75" customHeight="1">
+    <row r="149" spans="1:11" ht="12">
       <c r="A149" s="108" t="s">
         <v>53</v>
       </c>
@@ -5760,7 +6681,7 @@
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
     </row>
-    <row r="150" spans="1:11" ht="15.75" customHeight="1">
+    <row r="150" spans="1:11" ht="12">
       <c r="A150" s="43" t="s">
         <v>158</v>
       </c>
@@ -5785,7 +6706,7 @@
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
     </row>
-    <row r="151" spans="1:11" ht="15.75" customHeight="1">
+    <row r="151" spans="1:11" ht="12">
       <c r="A151" s="43" t="s">
         <v>159</v>
       </c>
@@ -5810,7 +6731,7 @@
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
     </row>
-    <row r="152" spans="1:11" ht="15.75" customHeight="1">
+    <row r="152" spans="1:11" ht="12">
       <c r="A152" s="43" t="s">
         <v>75</v>
       </c>
@@ -5835,7 +6756,7 @@
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
     </row>
-    <row r="153" spans="1:11" ht="15.75" customHeight="1">
+    <row r="153" spans="1:11" ht="12">
       <c r="A153" s="43" t="s">
         <v>138</v>
       </c>
@@ -5860,7 +6781,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
     </row>
-    <row r="154" spans="1:11" ht="15.75" customHeight="1">
+    <row r="154" spans="1:11" ht="12">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -5873,7 +6794,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
     </row>
-    <row r="155" spans="1:11" ht="15.75" customHeight="1">
+    <row r="155" spans="1:11" ht="48">
       <c r="A155" s="35" t="s">
         <v>250</v>
       </c>
@@ -5894,7 +6815,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
     </row>
-    <row r="156" spans="1:11" ht="15.75" customHeight="1">
+    <row r="156" spans="1:11" ht="12">
       <c r="A156" s="36" t="s">
         <v>10</v>
       </c>
@@ -5923,7 +6844,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
     </row>
-    <row r="157" spans="1:11" ht="15.75" customHeight="1">
+    <row r="157" spans="1:11" ht="12">
       <c r="A157" s="111" t="s">
         <v>14</v>
       </c>
@@ -5952,7 +6873,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
     </row>
-    <row r="158" spans="1:11" ht="15.75" customHeight="1">
+    <row r="158" spans="1:11" ht="12">
       <c r="A158" s="64" t="s">
         <v>16</v>
       </c>
@@ -5979,7 +6900,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="2"/>
     </row>
-    <row r="159" spans="1:11" ht="15.75" customHeight="1">
+    <row r="159" spans="1:11" ht="12">
       <c r="A159" s="66" t="s">
         <v>26</v>
       </c>
@@ -6003,7 +6924,7 @@
       <c r="J159" s="2"/>
       <c r="K159" s="2"/>
     </row>
-    <row r="160" spans="1:11" ht="15.75" customHeight="1">
+    <row r="160" spans="1:11" ht="12">
       <c r="A160" s="55" t="s">
         <v>180</v>
       </c>
@@ -6028,7 +6949,7 @@
       <c r="J160" s="2"/>
       <c r="K160" s="2"/>
     </row>
-    <row r="161" spans="1:12" ht="15.75" customHeight="1">
+    <row r="161" spans="1:12" ht="12">
       <c r="A161" s="55" t="s">
         <v>183</v>
       </c>
@@ -6053,7 +6974,7 @@
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
     </row>
-    <row r="162" spans="1:12" ht="15.75" customHeight="1">
+    <row r="162" spans="1:12" ht="24">
       <c r="A162" s="55" t="s">
         <v>185</v>
       </c>
@@ -6078,7 +6999,7 @@
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
     </row>
-    <row r="163" spans="1:12" ht="15.75" customHeight="1">
+    <row r="163" spans="1:12" ht="24">
       <c r="A163" s="55" t="s">
         <v>187</v>
       </c>
@@ -6103,7 +7024,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
     </row>
-    <row r="164" spans="1:12" ht="15.75" customHeight="1">
+    <row r="164" spans="1:12" ht="24">
       <c r="A164" s="55" t="s">
         <v>192</v>
       </c>
@@ -6128,7 +7049,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
     </row>
-    <row r="165" spans="1:12" ht="15.75" customHeight="1">
+    <row r="165" spans="1:12" ht="24">
       <c r="A165" s="55" t="s">
         <v>194</v>
       </c>
@@ -6153,7 +7074,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="2"/>
     </row>
-    <row r="166" spans="1:12" ht="15.75" customHeight="1">
+    <row r="166" spans="1:12" ht="24">
       <c r="A166" s="55" t="s">
         <v>196</v>
       </c>
@@ -6178,7 +7099,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
     </row>
-    <row r="167" spans="1:12" ht="15.75" customHeight="1">
+    <row r="167" spans="1:12" ht="12">
       <c r="A167" s="55" t="s">
         <v>198</v>
       </c>
@@ -6197,7 +7118,7 @@
       <c r="J167" s="2"/>
       <c r="K167" s="2"/>
     </row>
-    <row r="168" spans="1:12" ht="15.75" customHeight="1">
+    <row r="168" spans="1:12" ht="24">
       <c r="A168" s="64" t="s">
         <v>263</v>
       </c>
@@ -6214,15 +7135,15 @@
       <c r="J168" s="2"/>
       <c r="K168" s="2"/>
     </row>
-    <row r="169" spans="1:12" ht="15.75" customHeight="1">
+    <row r="169" spans="1:12" ht="12">
       <c r="D169" s="101"/>
       <c r="I169" s="101"/>
     </row>
-    <row r="170" spans="1:12" ht="15.75" customHeight="1">
+    <row r="170" spans="1:12" ht="12">
       <c r="D170" s="101"/>
       <c r="I170" s="101"/>
     </row>
-    <row r="171" spans="1:12" ht="15.75" customHeight="1">
+    <row r="171" spans="1:12" ht="144">
       <c r="A171" s="32" t="s">
         <v>265</v>
       </c>
@@ -6239,14 +7160,14 @@
       <c r="H171" s="55" t="s">
         <v>267</v>
       </c>
-      <c r="I171" s="145" t="s">
+      <c r="I171" s="137" t="s">
         <v>318</v>
       </c>
       <c r="J171" s="43"/>
       <c r="K171" s="43"/>
       <c r="L171" s="2"/>
     </row>
-    <row r="172" spans="1:12" ht="15.75" customHeight="1">
+    <row r="172" spans="1:12" ht="12">
       <c r="A172" s="36" t="s">
         <v>10</v>
       </c>
@@ -6276,7 +7197,7 @@
       <c r="K172" s="43"/>
       <c r="L172" s="2"/>
     </row>
-    <row r="173" spans="1:12" ht="15.75" customHeight="1">
+    <row r="173" spans="1:12" ht="12">
       <c r="A173" s="38" t="s">
         <v>14</v>
       </c>
@@ -6306,7 +7227,7 @@
       <c r="K173" s="43"/>
       <c r="L173" s="43"/>
     </row>
-    <row r="174" spans="1:12" ht="15.75" customHeight="1">
+    <row r="174" spans="1:12" ht="12">
       <c r="A174" s="108" t="s">
         <v>178</v>
       </c>
@@ -6334,7 +7255,7 @@
       <c r="K174" s="2"/>
       <c r="L174" s="2"/>
     </row>
-    <row r="175" spans="1:12" ht="15.75" customHeight="1">
+    <row r="175" spans="1:12" ht="12">
       <c r="A175" s="108" t="s">
         <v>169</v>
       </c>
@@ -6362,7 +7283,7 @@
       <c r="K175" s="2"/>
       <c r="L175" s="2"/>
     </row>
-    <row r="176" spans="1:12" ht="15.75" customHeight="1">
+    <row r="176" spans="1:12" ht="12">
       <c r="A176" s="43" t="s">
         <v>173</v>
       </c>
@@ -6376,10 +7297,10 @@
       <c r="F176" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="G176" s="136" t="s">
+      <c r="G176" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="H176" s="135"/>
+      <c r="H176" s="139"/>
       <c r="I176" s="33" t="s">
         <v>272</v>
       </c>
@@ -6387,7 +7308,7 @@
       <c r="K176" s="2"/>
       <c r="L176" s="2"/>
     </row>
-    <row r="177" spans="1:12" ht="15.75" customHeight="1">
+    <row r="177" spans="1:12" ht="12">
       <c r="A177" s="43" t="s">
         <v>177</v>
       </c>
@@ -6401,10 +7322,10 @@
       <c r="F177" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="G177" s="136" t="s">
+      <c r="G177" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H177" s="135"/>
+      <c r="H177" s="139"/>
       <c r="I177" s="33" t="s">
         <v>273</v>
       </c>
@@ -6412,7 +7333,7 @@
       <c r="K177" s="2"/>
       <c r="L177" s="2"/>
     </row>
-    <row r="178" spans="1:12" ht="15.75" customHeight="1">
+    <row r="178" spans="1:12" ht="12">
       <c r="A178" s="43" t="s">
         <v>179</v>
       </c>
@@ -6426,10 +7347,10 @@
       <c r="F178" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="G178" s="136" t="s">
+      <c r="G178" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H178" s="135"/>
+      <c r="H178" s="139"/>
       <c r="I178" s="33" t="s">
         <v>274</v>
       </c>
@@ -6437,7 +7358,7 @@
       <c r="K178" s="2"/>
       <c r="L178" s="2"/>
     </row>
-    <row r="179" spans="1:12" ht="15.75" customHeight="1">
+    <row r="179" spans="1:12" ht="12">
       <c r="A179" s="43" t="s">
         <v>182</v>
       </c>
@@ -6451,10 +7372,10 @@
       <c r="F179" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="G179" s="136" t="s">
+      <c r="G179" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H179" s="135"/>
+      <c r="H179" s="139"/>
       <c r="I179" s="33" t="s">
         <v>275</v>
       </c>
@@ -6462,7 +7383,7 @@
       <c r="K179" s="2"/>
       <c r="L179" s="2"/>
     </row>
-    <row r="180" spans="1:12" ht="15.75" customHeight="1">
+    <row r="180" spans="1:12" ht="24">
       <c r="A180" s="43" t="s">
         <v>184</v>
       </c>
@@ -6476,10 +7397,10 @@
       <c r="F180" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="G180" s="136" t="s">
+      <c r="G180" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H180" s="135"/>
+      <c r="H180" s="139"/>
       <c r="I180" s="57" t="s">
         <v>277</v>
       </c>
@@ -6487,7 +7408,7 @@
       <c r="K180" s="2"/>
       <c r="L180" s="2"/>
     </row>
-    <row r="181" spans="1:12" ht="15.75" customHeight="1">
+    <row r="181" spans="1:12" ht="12">
       <c r="A181" s="43" t="s">
         <v>186</v>
       </c>
@@ -6501,10 +7422,10 @@
       <c r="F181" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="G181" s="136" t="s">
+      <c r="G181" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H181" s="135"/>
+      <c r="H181" s="139"/>
       <c r="I181" s="33" t="s">
         <v>278</v>
       </c>
@@ -6512,7 +7433,7 @@
       <c r="K181" s="2"/>
       <c r="L181" s="2"/>
     </row>
-    <row r="182" spans="1:12" ht="15.75" customHeight="1">
+    <row r="182" spans="1:12" ht="12">
       <c r="A182" s="64" t="s">
         <v>191</v>
       </c>
@@ -6527,10 +7448,10 @@
       <c r="F182" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="G182" s="136" t="s">
+      <c r="G182" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H182" s="135"/>
+      <c r="H182" s="139"/>
       <c r="I182" s="33" t="s">
         <v>280</v>
       </c>
@@ -6538,7 +7459,7 @@
       <c r="K182" s="2"/>
       <c r="L182" s="2"/>
     </row>
-    <row r="183" spans="1:12" ht="15.75" customHeight="1">
+    <row r="183" spans="1:12" ht="12">
       <c r="A183" s="64" t="s">
         <v>193</v>
       </c>
@@ -6553,10 +7474,10 @@
       <c r="F183" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="G183" s="136" t="s">
+      <c r="G183" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H183" s="135"/>
+      <c r="H183" s="139"/>
       <c r="I183" s="33" t="s">
         <v>282</v>
       </c>
@@ -6564,7 +7485,7 @@
       <c r="K183" s="2"/>
       <c r="L183" s="2"/>
     </row>
-    <row r="184" spans="1:12" ht="15.75" customHeight="1">
+    <row r="184" spans="1:12" ht="12">
       <c r="A184" s="43" t="s">
         <v>195</v>
       </c>
@@ -6578,10 +7499,10 @@
       <c r="F184" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="G184" s="136" t="s">
+      <c r="G184" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H184" s="135"/>
+      <c r="H184" s="139"/>
       <c r="I184" s="33" t="s">
         <v>283</v>
       </c>
@@ -6589,7 +7510,7 @@
       <c r="K184" s="2"/>
       <c r="L184" s="2"/>
     </row>
-    <row r="185" spans="1:12" ht="15.75" customHeight="1">
+    <row r="185" spans="1:12" ht="12">
       <c r="A185" s="43" t="s">
         <v>197</v>
       </c>
@@ -6603,10 +7524,10 @@
       <c r="F185" s="54" t="s">
         <v>201</v>
       </c>
-      <c r="G185" s="136" t="s">
+      <c r="G185" s="138" t="s">
         <v>64</v>
       </c>
-      <c r="H185" s="135"/>
+      <c r="H185" s="139"/>
       <c r="I185" s="33" t="s">
         <v>284</v>
       </c>
@@ -6614,7 +7535,7 @@
       <c r="K185" s="2"/>
       <c r="L185" s="2"/>
     </row>
-    <row r="186" spans="1:12" ht="15.75" customHeight="1">
+    <row r="186" spans="1:12" ht="12">
       <c r="A186" s="43" t="s">
         <v>199</v>
       </c>
@@ -6630,7 +7551,7 @@
       <c r="K186" s="2"/>
       <c r="L186" s="2"/>
     </row>
-    <row r="187" spans="1:12" ht="15.75" customHeight="1">
+    <row r="187" spans="1:12" ht="12">
       <c r="A187" s="43" t="s">
         <v>201</v>
       </c>
@@ -6646,7 +7567,7 @@
       <c r="K187" s="2"/>
       <c r="L187" s="2"/>
     </row>
-    <row r="188" spans="1:12" ht="15.75" customHeight="1">
+    <row r="188" spans="1:12" ht="12">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -6660,7 +7581,7 @@
       <c r="K188" s="2"/>
       <c r="L188" s="2"/>
     </row>
-    <row r="189" spans="1:12" ht="15.75" customHeight="1">
+    <row r="189" spans="1:12" ht="132">
       <c r="A189" s="32" t="s">
         <v>285</v>
       </c>
@@ -6678,7 +7599,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="190" spans="1:12" ht="15.75" customHeight="1">
+    <row r="190" spans="1:12" ht="12">
       <c r="A190" s="36" t="s">
         <v>10</v>
       </c>
@@ -6704,7 +7625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="15.75" customHeight="1">
+    <row r="191" spans="1:12" ht="12">
       <c r="A191" s="123"/>
       <c r="B191" s="123"/>
       <c r="C191" s="9"/>
@@ -6714,14 +7635,14 @@
       <c r="H191" s="2"/>
       <c r="I191" s="101"/>
     </row>
-    <row r="192" spans="1:12" ht="15.75" customHeight="1">
+    <row r="192" spans="1:12" ht="12">
       <c r="A192" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B192" s="136" t="s">
+      <c r="B192" s="138" t="s">
         <v>129</v>
       </c>
-      <c r="C192" s="135"/>
+      <c r="C192" s="139"/>
       <c r="D192" s="107" t="s">
         <v>18</v>
       </c>
@@ -6738,29 +7659,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="15.75" customHeight="1">
+    <row r="193" spans="1:9" ht="12">
       <c r="A193" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="B193" s="139" t="s">
+      <c r="B193" s="145" t="s">
         <v>157</v>
       </c>
-      <c r="C193" s="135"/>
+      <c r="C193" s="139"/>
       <c r="D193" s="128" t="s">
         <v>288</v>
       </c>
       <c r="F193" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G193" s="136" t="s">
+      <c r="G193" s="138" t="s">
         <v>129</v>
       </c>
-      <c r="H193" s="135"/>
+      <c r="H193" s="139"/>
       <c r="I193" s="107" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.75" customHeight="1">
+    <row r="194" spans="1:9" ht="12">
       <c r="A194" s="43" t="s">
         <v>29</v>
       </c>
@@ -6774,15 +7695,15 @@
       <c r="F194" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="G194" s="136" t="s">
+      <c r="G194" s="138" t="s">
         <v>157</v>
       </c>
-      <c r="H194" s="135"/>
+      <c r="H194" s="139"/>
       <c r="I194" s="129" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="15.75" customHeight="1">
+    <row r="195" spans="1:9" ht="12">
       <c r="A195" s="43" t="s">
         <v>37</v>
       </c>
@@ -6804,7 +7725,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.75" customHeight="1">
+    <row r="196" spans="1:9" ht="12">
       <c r="A196" s="43" t="s">
         <v>167</v>
       </c>
@@ -6826,7 +7747,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.75" customHeight="1">
+    <row r="197" spans="1:9" ht="12">
       <c r="A197" s="43" t="s">
         <v>168</v>
       </c>
@@ -6848,7 +7769,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="15.75" customHeight="1">
+    <row r="198" spans="1:9" ht="12">
       <c r="A198" s="108" t="s">
         <v>169</v>
       </c>
@@ -6870,7 +7791,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.75" customHeight="1">
+    <row r="199" spans="1:9" ht="12">
       <c r="A199" s="43" t="s">
         <v>101</v>
       </c>
@@ -6892,14 +7813,14 @@
         <v>293</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="15.75" customHeight="1">
+    <row r="200" spans="1:9" ht="24">
       <c r="A200" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="B200" s="136" t="s">
+      <c r="B200" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="C200" s="135"/>
+      <c r="C200" s="139"/>
       <c r="D200" s="107" t="s">
         <v>295</v>
       </c>
@@ -6914,7 +7835,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="15.75" customHeight="1">
+    <row r="201" spans="1:9" ht="24">
       <c r="A201" s="43" t="s">
         <v>177</v>
       </c>
@@ -6928,15 +7849,15 @@
       <c r="F201" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="G201" s="136" t="s">
+      <c r="G201" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="H201" s="135"/>
+      <c r="H201" s="139"/>
       <c r="I201" s="107" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="15.75" customHeight="1">
+    <row r="202" spans="1:9" ht="24">
       <c r="A202" s="43" t="s">
         <v>179</v>
       </c>
@@ -6958,14 +7879,14 @@
         <v>296</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="15.75" customHeight="1">
+    <row r="203" spans="1:9" ht="24">
       <c r="A203" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="B203" s="136" t="s">
+      <c r="B203" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="C203" s="135"/>
+      <c r="C203" s="139"/>
       <c r="D203" s="107" t="s">
         <v>298</v>
       </c>
@@ -6980,51 +7901,51 @@
         <v>297</v>
       </c>
     </row>
-    <row r="204" spans="1:9" ht="15.75" customHeight="1">
+    <row r="204" spans="1:9" ht="24">
       <c r="A204" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="B204" s="136" t="s">
+      <c r="B204" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="C204" s="135"/>
+      <c r="C204" s="139"/>
       <c r="D204" s="107" t="s">
         <v>44</v>
       </c>
       <c r="F204" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="G204" s="136" t="s">
+      <c r="G204" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="H204" s="135"/>
+      <c r="H204" s="139"/>
       <c r="I204" s="107" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="15.75" customHeight="1">
+    <row r="205" spans="1:9" ht="24">
       <c r="A205" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="B205" s="136" t="s">
+      <c r="B205" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="C205" s="135"/>
+      <c r="C205" s="139"/>
       <c r="D205" s="107" t="s">
         <v>299</v>
       </c>
       <c r="F205" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="G205" s="136" t="s">
+      <c r="G205" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="H205" s="135"/>
+      <c r="H205" s="139"/>
       <c r="I205" s="107" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="15.75" customHeight="1">
+    <row r="206" spans="1:9" ht="24">
       <c r="A206" s="43" t="s">
         <v>191</v>
       </c>
@@ -7038,15 +7959,15 @@
       <c r="F206" s="43" t="s">
         <v>186</v>
       </c>
-      <c r="G206" s="136" t="s">
+      <c r="G206" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="H206" s="135"/>
+      <c r="H206" s="139"/>
       <c r="I206" s="107" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="15.75" customHeight="1">
+    <row r="207" spans="1:9" ht="24">
       <c r="A207" s="43" t="s">
         <v>193</v>
       </c>
@@ -7068,7 +7989,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="15.75" customHeight="1">
+    <row r="208" spans="1:9" ht="24">
       <c r="A208" s="43" t="s">
         <v>195</v>
       </c>
@@ -7090,7 +8011,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.75" customHeight="1">
+    <row r="209" spans="1:9" ht="24">
       <c r="A209" s="43" t="s">
         <v>197</v>
       </c>
@@ -7112,7 +8033,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="15.75" customHeight="1">
+    <row r="210" spans="1:9" ht="24">
       <c r="A210" s="43" t="s">
         <v>199</v>
       </c>
@@ -7134,7 +8055,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="15.75" customHeight="1">
+    <row r="211" spans="1:9" ht="24">
       <c r="A211" s="43" t="s">
         <v>201</v>
       </c>
@@ -7156,7 +8077,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="15.75" customHeight="1">
+    <row r="212" spans="1:9" ht="36">
       <c r="A212" s="44" t="s">
         <v>306</v>
       </c>
@@ -7178,7 +8099,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="213" spans="1:9" ht="15.75" customHeight="1">
+    <row r="213" spans="1:9" ht="36">
       <c r="A213" s="66" t="s">
         <v>178</v>
       </c>
@@ -7200,14 +8121,14 @@
         <v>308</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="15.75" customHeight="1">
+    <row r="214" spans="1:9" ht="12">
       <c r="A214" s="64" t="s">
         <v>309</v>
       </c>
-      <c r="B214" s="137" t="s">
+      <c r="B214" s="142" t="s">
         <v>238</v>
       </c>
-      <c r="C214" s="135"/>
+      <c r="C214" s="139"/>
       <c r="D214" s="81" t="s">
         <v>310</v>
       </c>
@@ -7222,7 +8143,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="15.75" customHeight="1">
+    <row r="215" spans="1:9" ht="24">
       <c r="A215" s="43" t="s">
         <v>203</v>
       </c>
@@ -7236,44 +8157,44 @@
       <c r="F215" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="G215" s="136" t="s">
+      <c r="G215" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="H215" s="135"/>
+      <c r="H215" s="139"/>
       <c r="I215" s="107" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="15.75" customHeight="1">
+    <row r="216" spans="1:9" ht="24">
       <c r="A216" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="B216" s="136" t="s">
+      <c r="B216" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="C216" s="135"/>
+      <c r="C216" s="139"/>
       <c r="D216" s="107" t="s">
         <v>312</v>
       </c>
       <c r="F216" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="G216" s="136" t="s">
+      <c r="G216" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="H216" s="135"/>
+      <c r="H216" s="139"/>
       <c r="I216" s="107" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="217" spans="1:9" ht="15.75" customHeight="1">
+    <row r="217" spans="1:9" ht="12">
       <c r="A217" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B217" s="136" t="s">
+      <c r="B217" s="138" t="s">
         <v>114</v>
       </c>
-      <c r="C217" s="135"/>
+      <c r="C217" s="139"/>
       <c r="D217" s="107" t="s">
         <v>313</v>
       </c>
@@ -7288,7 +8209,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="15.75" customHeight="1">
+    <row r="218" spans="1:9" ht="12">
       <c r="A218" s="43" t="s">
         <v>205</v>
       </c>
@@ -11152,30 +12073,24 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="G132:H132"/>
-    <mergeCell ref="G131:H131"/>
-    <mergeCell ref="G181:H181"/>
-    <mergeCell ref="G182:H182"/>
-    <mergeCell ref="G185:H185"/>
-    <mergeCell ref="G178:H178"/>
-    <mergeCell ref="G179:H179"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="G215:H215"/>
+    <mergeCell ref="B205:C205"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="B192:C192"/>
+    <mergeCell ref="B193:C193"/>
+    <mergeCell ref="B204:C204"/>
     <mergeCell ref="B217:C217"/>
     <mergeCell ref="B200:C200"/>
     <mergeCell ref="G180:H180"/>
@@ -11192,26 +12107,32 @@
     <mergeCell ref="G204:H204"/>
     <mergeCell ref="G201:H201"/>
     <mergeCell ref="G216:H216"/>
-    <mergeCell ref="G215:H215"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B203:C203"/>
-    <mergeCell ref="B192:C192"/>
-    <mergeCell ref="B193:C193"/>
-    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="A54:B54"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="G71:H71"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G132:H132"/>
+    <mergeCell ref="G131:H131"/>
+    <mergeCell ref="G181:H181"/>
+    <mergeCell ref="G182:H182"/>
+    <mergeCell ref="G185:H185"/>
+    <mergeCell ref="G178:H178"/>
+    <mergeCell ref="G179:H179"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11225,10 +12146,743 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R146"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="13" width="14.5" style="134"/>
+    <col min="14" max="14" width="19.6640625" style="134" customWidth="1"/>
+    <col min="15" max="16384" width="14.5" style="134"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" ht="12">
+      <c r="N2" s="78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="12">
+      <c r="C3" s="136" t="s">
+        <v>315</v>
+      </c>
+      <c r="N3" s="149" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="12">
+      <c r="N4" s="150" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="12">
+      <c r="C5" s="136" t="s">
+        <v>316</v>
+      </c>
+      <c r="N5" s="77" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="12">
+      <c r="C6" s="136" t="s">
+        <v>317</v>
+      </c>
+      <c r="F6" s="148" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="12">
+      <c r="C7" s="134" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="152" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="12">
+      <c r="F8" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="135"/>
+    </row>
+    <row r="9" spans="1:14" ht="12">
+      <c r="A9" s="135"/>
+      <c r="F9" s="151" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="12">
+      <c r="F10" s="151" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="78" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="12">
+      <c r="F11" s="151" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="12">
+      <c r="F12" s="151" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="150" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="12">
+      <c r="F13" s="151" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" s="77" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="12">
+      <c r="F14" s="151" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="77" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="12">
+      <c r="F15" s="151" t="s">
+        <v>43</v>
+      </c>
+      <c r="N15" s="77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="12">
+      <c r="F16" s="153" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="152" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="12">
+      <c r="J17" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" s="135"/>
+    </row>
+    <row r="18" spans="1:14" ht="12">
+      <c r="J18" s="149" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="12">
+      <c r="H19" s="148" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="150" t="s">
+        <v>97</v>
+      </c>
+      <c r="N19" s="78" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="12">
+      <c r="H20" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="150" t="s">
+        <v>99</v>
+      </c>
+      <c r="N20" s="84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="12">
+      <c r="H21" s="151" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="150" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="12">
+      <c r="A22" s="135"/>
+      <c r="F22" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="151" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="150" t="s">
+        <v>107</v>
+      </c>
+      <c r="N22" s="77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="12">
+      <c r="F23" s="149" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="151" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="150" t="s">
+        <v>111</v>
+      </c>
+      <c r="N23" s="77" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="12">
+      <c r="F24" s="155" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="151" t="s">
+        <v>23</v>
+      </c>
+      <c r="J24" s="150" t="s">
+        <v>116</v>
+      </c>
+      <c r="N24" s="77" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="12">
+      <c r="F25" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="154" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="150" t="s">
+        <v>119</v>
+      </c>
+      <c r="N25" s="77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="12">
+      <c r="F26" s="77" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="150" t="s">
+        <v>120</v>
+      </c>
+      <c r="N26" s="152" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="12">
+      <c r="F27" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="J27" s="150" t="s">
+        <v>123</v>
+      </c>
+      <c r="N27" s="135"/>
+    </row>
+    <row r="28" spans="1:14" ht="12">
+      <c r="F28" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" s="150" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="12">
+      <c r="D29" s="135"/>
+      <c r="F29" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="J29" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="N29" s="78" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="12">
+      <c r="D30" s="78" t="s">
+        <v>241</v>
+      </c>
+      <c r="F30" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="J30" s="150" t="s">
+        <v>127</v>
+      </c>
+      <c r="N30" s="149" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="12">
+      <c r="D31" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31" s="82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="12">
+      <c r="D32" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="F32" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="J32" s="77" t="s">
+        <v>105</v>
+      </c>
+      <c r="N32" s="77" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" customHeight="1">
+      <c r="D33" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="F33" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="J33" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="N33" s="80" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" customHeight="1">
+      <c r="D34" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="82" t="s">
+        <v>72</v>
+      </c>
+      <c r="J34" s="150" t="s">
+        <v>130</v>
+      </c>
+      <c r="N34" s="135"/>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" customHeight="1">
+      <c r="D35" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="J35" s="150" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" customHeight="1">
+      <c r="F36" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="J36" s="150" t="s">
+        <v>136</v>
+      </c>
+      <c r="N36" s="78" t="s">
+        <v>230</v>
+      </c>
+      <c r="P36" s="135"/>
+    </row>
+    <row r="37" spans="1:18" ht="15.75" customHeight="1">
+      <c r="F37" s="82" t="s">
+        <v>80</v>
+      </c>
+      <c r="J37" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="N37" s="149" t="s">
+        <v>14</v>
+      </c>
+      <c r="P37" s="78" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="15.75" customHeight="1">
+      <c r="F38" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="J38" s="150" t="s">
+        <v>138</v>
+      </c>
+      <c r="N38" s="150" t="s">
+        <v>109</v>
+      </c>
+      <c r="P38" s="77" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" customHeight="1">
+      <c r="F39" s="82" t="s">
+        <v>84</v>
+      </c>
+      <c r="J39" s="77" t="s">
+        <v>29</v>
+      </c>
+      <c r="N39" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="P39" s="149" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="15.75" customHeight="1">
+      <c r="F40" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="J40" s="150" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40" s="80" t="s">
+        <v>113</v>
+      </c>
+      <c r="P40" s="77" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="15.75" customHeight="1">
+      <c r="F41" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="J41" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="L41" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="P41" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="R41" s="156"/>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" customHeight="1">
+      <c r="L42" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="P42" s="77" t="s">
+        <v>167</v>
+      </c>
+      <c r="R42" s="156"/>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" customHeight="1">
+      <c r="L43" s="149" t="s">
+        <v>14</v>
+      </c>
+      <c r="P43" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="R43" s="148" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="15.75" customHeight="1">
+      <c r="A44" s="135"/>
+      <c r="G44" s="78" t="s">
+        <v>250</v>
+      </c>
+      <c r="L44" s="150" t="s">
+        <v>97</v>
+      </c>
+      <c r="P44" s="151" t="s">
+        <v>169</v>
+      </c>
+      <c r="R44" s="84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" customHeight="1">
+      <c r="A45" s="135"/>
+      <c r="G45" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="L45" s="155" t="s">
+        <v>26</v>
+      </c>
+      <c r="P45" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="R45" s="151" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="15.75" customHeight="1">
+      <c r="G46" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="L46" s="77" t="s">
+        <v>101</v>
+      </c>
+      <c r="N46" s="78" t="s">
+        <v>265</v>
+      </c>
+      <c r="P46" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="R46" s="151" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" customHeight="1">
+      <c r="G47" s="150" t="s">
+        <v>16</v>
+      </c>
+      <c r="L47" s="157" t="s">
+        <v>134</v>
+      </c>
+      <c r="N47" s="149" t="s">
+        <v>14</v>
+      </c>
+      <c r="P47" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="R47" s="151" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="15.75" customHeight="1">
+      <c r="G48" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" s="157" t="s">
+        <v>136</v>
+      </c>
+      <c r="N48" s="86" t="s">
+        <v>178</v>
+      </c>
+      <c r="P48" s="77" t="s">
+        <v>179</v>
+      </c>
+      <c r="R48" s="151" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G49" s="82" t="s">
+        <v>180</v>
+      </c>
+      <c r="L49" s="77" t="s">
+        <v>113</v>
+      </c>
+      <c r="N49" s="86" t="s">
+        <v>169</v>
+      </c>
+      <c r="P49" s="77" t="s">
+        <v>182</v>
+      </c>
+      <c r="R49" s="151" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G50" s="82" t="s">
+        <v>183</v>
+      </c>
+      <c r="L50" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="N50" s="77" t="s">
+        <v>173</v>
+      </c>
+      <c r="P50" s="77" t="s">
+        <v>184</v>
+      </c>
+      <c r="R50" s="151" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G51" s="82" t="s">
+        <v>185</v>
+      </c>
+      <c r="L51" s="77" t="s">
+        <v>169</v>
+      </c>
+      <c r="N51" s="77" t="s">
+        <v>177</v>
+      </c>
+      <c r="P51" s="77" t="s">
+        <v>186</v>
+      </c>
+      <c r="R51" s="153" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G52" s="82" t="s">
+        <v>187</v>
+      </c>
+      <c r="L52" s="102" t="s">
+        <v>178</v>
+      </c>
+      <c r="N52" s="77" t="s">
+        <v>179</v>
+      </c>
+      <c r="P52" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="R52" s="156"/>
+    </row>
+    <row r="53" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G53" s="82" t="s">
+        <v>192</v>
+      </c>
+      <c r="N53" s="77" t="s">
+        <v>182</v>
+      </c>
+      <c r="P53" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="R53" s="156"/>
+    </row>
+    <row r="54" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G54" s="82" t="s">
+        <v>194</v>
+      </c>
+      <c r="N54" s="77" t="s">
+        <v>184</v>
+      </c>
+      <c r="P54" s="77" t="s">
+        <v>195</v>
+      </c>
+      <c r="R54" s="156"/>
+    </row>
+    <row r="55" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G55" s="82" t="s">
+        <v>196</v>
+      </c>
+      <c r="N55" s="77" t="s">
+        <v>186</v>
+      </c>
+      <c r="P55" s="77" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G56" s="82" t="s">
+        <v>198</v>
+      </c>
+      <c r="N56" s="150" t="s">
+        <v>191</v>
+      </c>
+      <c r="P56" s="77" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="7:18" ht="15.75" customHeight="1">
+      <c r="G57" s="152" t="s">
+        <v>263</v>
+      </c>
+      <c r="N57" s="150" t="s">
+        <v>193</v>
+      </c>
+      <c r="P57" s="77" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="7:18" ht="15.75" customHeight="1">
+      <c r="N58" s="77" t="s">
+        <v>195</v>
+      </c>
+      <c r="P58" s="158" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="7:18" ht="15.75" customHeight="1">
+      <c r="N59" s="77" t="s">
+        <v>197</v>
+      </c>
+      <c r="P59" s="159" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="7:18" ht="15.75" customHeight="1">
+      <c r="N60" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="P60" s="150" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="61" spans="7:18" ht="15.75" customHeight="1">
+      <c r="N61" s="80" t="s">
+        <v>201</v>
+      </c>
+      <c r="P61" s="77" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="7:18" ht="15.75" customHeight="1">
+      <c r="N62" s="135"/>
+      <c r="P62" s="77" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="63" spans="7:18" ht="15.75" customHeight="1">
+      <c r="P63" s="77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="7:18" ht="15.75" customHeight="1">
+      <c r="P64" s="80" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="12">
+      <c r="A72" s="135"/>
+    </row>
+    <row r="85" spans="1:1" ht="12">
+      <c r="A85" s="135"/>
+    </row>
+    <row r="126" spans="1:1" ht="12">
+      <c r="A126" s="135"/>
+    </row>
+    <row r="137" spans="1:1" ht="12">
+      <c r="A137" s="135"/>
+    </row>
+    <row r="146" spans="1:1" ht="12">
+      <c r="A146" s="135"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -11238,7 +12892,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="5:12" ht="15.75" customHeight="1">
-      <c r="E3" s="144" t="s">
+      <c r="E3" s="136" t="s">
         <v>315</v>
       </c>
     </row>
@@ -11248,7 +12902,7 @@
       </c>
     </row>
     <row r="5" spans="5:12" ht="15.75" customHeight="1">
-      <c r="E5" s="144" t="s">
+      <c r="E5" s="136" t="s">
         <v>316</v>
       </c>
       <c r="L5" s="70" t="s">
@@ -11256,7 +12910,7 @@
       </c>
     </row>
     <row r="6" spans="5:12" ht="15.75" customHeight="1">
-      <c r="E6" s="144" t="s">
+      <c r="E6" s="136" t="s">
         <v>317</v>
       </c>
       <c r="L6" s="71" t="s">
@@ -11561,8 +13215,8 @@
       </c>
     </row>
     <row r="38" spans="6:15" ht="15.75" customHeight="1">
-      <c r="O38" s="86" t="s">
-        <v>169</v>
+      <c r="O38" s="77" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="6:15" ht="15.75" customHeight="1">
@@ -11573,7 +13227,7 @@
         <v>170</v>
       </c>
       <c r="O39" s="77" t="s">
-        <v>101</v>
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="6:15" ht="15.75" customHeight="1">
@@ -11587,7 +13241,7 @@
         <v>172</v>
       </c>
       <c r="O40" s="77" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="6:15" ht="15.75" customHeight="1">
@@ -11601,7 +13255,7 @@
         <v>176</v>
       </c>
       <c r="O41" s="77" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="6:15" ht="15.75" customHeight="1">
@@ -11615,7 +13269,7 @@
         <v>178</v>
       </c>
       <c r="O42" s="77" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="6:15" ht="15.75" customHeight="1">
@@ -11629,7 +13283,7 @@
         <v>169</v>
       </c>
       <c r="O43" s="77" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="6:15" ht="15.75" customHeight="1">
@@ -11643,7 +13297,7 @@
         <v>173</v>
       </c>
       <c r="O44" s="77" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="6:15" ht="15.75" customHeight="1">
@@ -11657,7 +13311,7 @@
         <v>177</v>
       </c>
       <c r="O45" s="77" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="46" spans="6:15" ht="15.75" customHeight="1">
@@ -11671,7 +13325,7 @@
         <v>179</v>
       </c>
       <c r="O46" s="77" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="6:15" ht="15.75" customHeight="1">
@@ -11682,7 +13336,7 @@
         <v>182</v>
       </c>
       <c r="O47" s="77" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="6:15" ht="15.75" customHeight="1">
@@ -11693,7 +13347,7 @@
         <v>184</v>
       </c>
       <c r="O48" s="77" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="3:15" ht="15.75" customHeight="1">
@@ -11704,7 +13358,7 @@
         <v>186</v>
       </c>
       <c r="O49" s="77" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="50" spans="3:15" ht="15.75" customHeight="1">
@@ -11716,7 +13370,7 @@
         <v>195</v>
       </c>
       <c r="O50" s="77" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="3:15" ht="15.75" customHeight="1">
@@ -11725,15 +13379,15 @@
         <v>197</v>
       </c>
       <c r="O51" s="77" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="3:15" ht="15.75" customHeight="1">
       <c r="M52" s="77" t="s">
         <v>199</v>
       </c>
-      <c r="O52" s="76" t="s">
-        <v>178</v>
+      <c r="O52" s="77" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="3:15" ht="15.75" customHeight="1">
@@ -11741,24 +13395,14 @@
         <v>201</v>
       </c>
       <c r="O53" s="77" t="s">
-        <v>203</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="3:15" ht="15.75" customHeight="1">
       <c r="M54" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="O54" s="77" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="55" spans="3:15" ht="15.75" customHeight="1">
-      <c r="O55" s="77" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="56" spans="3:15" ht="15.75" customHeight="1">
-      <c r="O56" s="80" t="s">
+      <c r="O54" s="80" t="s">
         <v>205</v>
       </c>
     </row>

</xml_diff>